<commit_message>
Added conductance calculations and calibration
</commit_message>
<xml_diff>
--- a/00_additional_data/COS_timing.xlsx
+++ b/00_additional_data/COS_timing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="15">
   <si>
     <t>date</t>
   </si>
@@ -392,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1078,7 +1078,110 @@
         <v>44501.03466435185</v>
       </c>
     </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="1">
+        <v>44236</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>45</v>
+      </c>
+      <c r="E38">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="1">
+        <v>44236</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="1">
+        <v>44236</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="1">
+        <v>44236</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>12</v>
+      </c>
+      <c r="E41">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="1">
+        <v>44236</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42">
+        <v>20</v>
+      </c>
+      <c r="E42">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="1">
+        <v>44236</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43">
+        <v>35</v>
+      </c>
+      <c r="E43">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed small error with "calibrated" columns
</commit_message>
<xml_diff>
--- a/00_additional_data/COS_timing.xlsx
+++ b/00_additional_data/COS_timing.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\python\_rafat_laser\00_additional_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\_Data\202008-now - Laser chambers - Rafat\00_additional_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="15">
   <si>
     <t>date</t>
   </si>
@@ -107,11 +107,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E45" sqref="A24:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -685,7 +687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>44056</v>
       </c>
@@ -702,7 +704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>44056</v>
       </c>
@@ -719,7 +721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>44056</v>
       </c>
@@ -736,7 +738,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
         <v>44071</v>
       </c>
@@ -752,8 +754,14 @@
       <c r="E20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
         <v>44071</v>
       </c>
@@ -769,8 +777,14 @@
       <c r="E21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G21" s="1"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1">
         <v>44071</v>
       </c>
@@ -786,8 +800,14 @@
       <c r="E22">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G22" s="1"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1">
         <v>44071</v>
       </c>
@@ -803,385 +823,612 @@
       <c r="E23">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="1">
+      <c r="G23" s="1"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="4">
         <v>44071</v>
       </c>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24">
+      <c r="B24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="5">
         <v>10</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="5">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="1">
+      <c r="G24" s="1"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="4">
+        <v>44100</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="2">
+        <v>55</v>
+      </c>
+      <c r="E25" s="2">
+        <v>59</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="4">
+        <v>44100</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>7</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="4">
+        <v>44100</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2">
+        <v>8</v>
+      </c>
+      <c r="E27" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="4">
+        <v>44100</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="2">
+        <v>12</v>
+      </c>
+      <c r="E28" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="4">
+        <v>44100</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2">
+        <v>16</v>
+      </c>
+      <c r="E29" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="4">
+        <v>44100</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="2">
+        <v>26</v>
+      </c>
+      <c r="E30" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="4">
         <v>44105</v>
       </c>
-      <c r="B25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25">
+      <c r="B31" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="5">
         <v>0</v>
       </c>
-      <c r="E25">
+      <c r="E31" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="1">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="4">
         <v>44105</v>
       </c>
-      <c r="B26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26">
-        <v>8</v>
-      </c>
-      <c r="E26">
+      <c r="B32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="5">
+        <v>8</v>
+      </c>
+      <c r="E32" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="1">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="4">
         <v>44105</v>
       </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27">
+      <c r="B33" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="5">
         <v>12</v>
       </c>
-      <c r="E27">
+      <c r="E33" s="5">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="1">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="4">
         <v>44105</v>
       </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28">
+      <c r="B34" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="5">
         <v>20</v>
       </c>
-      <c r="E28">
+      <c r="E34" s="5">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="1">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="4">
         <v>44105</v>
       </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29">
+      <c r="B35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="5">
         <v>24</v>
       </c>
-      <c r="E29">
+      <c r="E35" s="5">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="1">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="4">
         <v>44105</v>
       </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B36" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D30">
+      <c r="D36" s="5">
         <v>28</v>
       </c>
-      <c r="E30">
+      <c r="E36" s="5">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="1">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="4">
         <v>44105</v>
       </c>
-      <c r="B31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D31">
+      <c r="D37" s="5">
         <v>29</v>
       </c>
-      <c r="E31">
+      <c r="E37" s="5">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="1">
-        <v>44136</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="4">
+        <v>44106</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="2">
         <v>45</v>
       </c>
-      <c r="E32">
+      <c r="E38" s="2">
         <v>49</v>
       </c>
-      <c r="G32" s="3">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="4">
+        <v>44106</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="4">
+        <v>44106</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="2">
+        <v>8</v>
+      </c>
+      <c r="E40" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="4">
+        <v>44106</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="2">
+        <v>12</v>
+      </c>
+      <c r="E41" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="4">
+        <v>44106</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="2">
+        <v>16</v>
+      </c>
+      <c r="E42" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="4">
+        <v>44106</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="2">
+        <v>26</v>
+      </c>
+      <c r="E43" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="4">
+        <v>44108</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="5">
+        <v>45</v>
+      </c>
+      <c r="E44" s="5">
+        <v>49</v>
+      </c>
+      <c r="G44" s="3">
         <v>44501.031886574077</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H44" s="3">
         <v>44501.03466435185</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="1">
-        <v>44136</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="4">
+        <v>44108</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="5">
         <v>0</v>
       </c>
-      <c r="E33">
+      <c r="E45" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G45" s="3">
         <v>44501</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H45" s="3">
         <v>44501.005208333336</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="1">
-        <v>44136</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34">
-        <v>8</v>
-      </c>
-      <c r="E34">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>8</v>
+      </c>
+      <c r="E46">
         <v>11</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G46" s="3">
         <v>44501.005902777775</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H46" s="3">
         <v>44501.008275462962</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="1">
-        <v>44136</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47">
         <v>12</v>
       </c>
-      <c r="E35">
+      <c r="E47">
         <v>19</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G47" s="3">
         <v>44501.008333333331</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H47" s="3">
         <v>44501.013541666667</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="1">
-        <v>44136</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48">
         <v>20</v>
       </c>
-      <c r="E36">
+      <c r="E48">
         <v>27</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G48" s="3">
         <v>44501.014236111114</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H48" s="3">
         <v>44501.019386574073</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="1">
-        <v>44136</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="1">
+        <v>44108</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49">
         <v>45</v>
       </c>
-      <c r="E37">
+      <c r="E49">
         <v>49</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G49" s="3">
         <v>44501.031886574077</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H49" s="3">
         <v>44501.03466435185</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="1">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="1">
         <v>44236</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38">
+      <c r="B50" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50">
         <v>45</v>
       </c>
-      <c r="E38">
+      <c r="E50">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="1">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="1">
         <v>44236</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39">
+      <c r="B51" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51">
         <v>0</v>
       </c>
-      <c r="E39">
+      <c r="E51">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="1">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="1">
         <v>44236</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40">
-        <v>8</v>
-      </c>
-      <c r="E40">
+      <c r="B52" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52">
+        <v>8</v>
+      </c>
+      <c r="E52">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="1">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="1">
         <v>44236</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41">
+      <c r="B53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53">
         <v>12</v>
       </c>
-      <c r="E41">
+      <c r="E53">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="1">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="1">
         <v>44236</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42">
+      <c r="B54" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54">
         <v>20</v>
       </c>
-      <c r="E42">
+      <c r="E54">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="1">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1">
         <v>44236</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43">
+      <c r="B55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55">
         <v>35</v>
       </c>
-      <c r="E43">
+      <c r="E55">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>